<commit_message>
Fixed the Work Packages on the RAM
</commit_message>
<xml_diff>
--- a/project_data_ram.xlsx
+++ b/project_data_ram.xlsx
@@ -62,8 +62,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fb4934"/>
-        <bgColor rgb="00fb4934"/>
+        <fgColor rgb="00BDAE93"/>
+        <bgColor rgb="00BDAE93"/>
       </patternFill>
     </fill>
     <fill>
@@ -98,20 +98,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0083a598"/>
-        <bgColor rgb="0083a598"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00b8bb26"/>
         <bgColor rgb="00b8bb26"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fe8019"/>
-        <bgColor rgb="00fe8019"/>
+        <fgColor rgb="00fb4934"/>
+        <bgColor rgb="00fb4934"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0083a598"/>
+        <bgColor rgb="0083a598"/>
       </patternFill>
     </fill>
     <fill>
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K127"/>
+  <dimension ref="A1:L130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,7 +534,7 @@
   <cols>
     <col width="54" customWidth="1" min="1" max="1"/>
     <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
     <col width="82" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
@@ -543,6 +543,7 @@
     <col width="7" customWidth="1" min="9" max="9"/>
     <col width="30" customWidth="1" min="10" max="10"/>
     <col width="35" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -666,67 +667,67 @@
       <c r="K4" s="4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Battery Research</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr"/>
-      <c r="D5" s="4" t="inlineStr"/>
-      <c r="E5" s="4" t="inlineStr"/>
-      <c r="F5" s="4" t="inlineStr"/>
-      <c r="G5" s="4" t="inlineStr"/>
-      <c r="H5" s="4" t="inlineStr"/>
-      <c r="I5" s="4" t="inlineStr"/>
-      <c r="J5" s="4" t="inlineStr"/>
-      <c r="K5" s="4" t="inlineStr"/>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="5" t="inlineStr"/>
+      <c r="E5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
+      <c r="H5" s="5" t="inlineStr"/>
+      <c r="I5" s="5" t="inlineStr"/>
+      <c r="J5" s="5" t="inlineStr"/>
+      <c r="K5" s="5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                Battery Types</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr"/>
-      <c r="D6" s="4" t="inlineStr"/>
-      <c r="E6" s="4" t="inlineStr"/>
-      <c r="F6" s="4" t="inlineStr"/>
-      <c r="G6" s="4" t="inlineStr"/>
-      <c r="H6" s="4" t="inlineStr"/>
-      <c r="I6" s="4" t="inlineStr"/>
-      <c r="J6" s="4" t="inlineStr"/>
-      <c r="K6" s="4" t="inlineStr"/>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr"/>
+      <c r="E6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
+      <c r="H6" s="5" t="inlineStr"/>
+      <c r="I6" s="5" t="inlineStr"/>
+      <c r="J6" s="5" t="inlineStr"/>
+      <c r="K6" s="5" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Lithium Ion</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr"/>
-      <c r="D7" s="4" t="inlineStr"/>
-      <c r="E7" s="4" t="inlineStr"/>
-      <c r="F7" s="4" t="inlineStr"/>
-      <c r="G7" s="4" t="inlineStr"/>
-      <c r="H7" s="4" t="inlineStr"/>
-      <c r="I7" s="4" t="inlineStr"/>
-      <c r="J7" s="4" t="inlineStr"/>
-      <c r="K7" s="4" t="inlineStr"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="5" t="inlineStr"/>
+      <c r="E7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="5" t="inlineStr"/>
+      <c r="H7" s="5" t="inlineStr"/>
+      <c r="I7" s="5" t="inlineStr"/>
+      <c r="J7" s="5" t="inlineStr"/>
+      <c r="K7" s="5" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
@@ -736,14 +737,10 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr"/>
       <c r="D8" s="5" t="inlineStr"/>
       <c r="E8" s="5" t="inlineStr"/>
       <c r="F8" s="5" t="inlineStr"/>
@@ -766,7 +763,7 @@
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>1.1.1.1.1.1.1</t>
         </is>
       </c>
       <c r="D9" s="7" t="inlineStr">
@@ -811,7 +808,7 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>1.1.1.1.1.1.2</t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
@@ -856,7 +853,7 @@
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>1.1.1.1.1.1.3</t>
         </is>
       </c>
       <c r="D11" s="7" t="inlineStr">
@@ -896,14 +893,10 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C12" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr"/>
       <c r="D12" s="5" t="inlineStr"/>
       <c r="E12" s="5" t="inlineStr"/>
       <c r="F12" s="5" t="inlineStr"/>
@@ -926,7 +919,7 @@
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>1.1.1.1.1.2.1</t>
         </is>
       </c>
       <c r="D13" s="7" t="inlineStr">
@@ -967,7 +960,7 @@
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>1.1.1.1.1.2.2</t>
         </is>
       </c>
       <c r="D14" s="7" t="inlineStr">
@@ -1008,7 +1001,7 @@
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>1.1.1.1.1.2.3</t>
         </is>
       </c>
       <c r="D15" s="7" t="inlineStr">
@@ -1037,25 +1030,25 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    LiFePO4</t>
         </is>
       </c>
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr"/>
-      <c r="D16" s="4" t="inlineStr"/>
-      <c r="E16" s="4" t="inlineStr"/>
-      <c r="F16" s="4" t="inlineStr"/>
-      <c r="G16" s="4" t="inlineStr"/>
-      <c r="H16" s="4" t="inlineStr"/>
-      <c r="I16" s="4" t="inlineStr"/>
-      <c r="J16" s="4" t="inlineStr"/>
-      <c r="K16" s="4" t="inlineStr"/>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr"/>
+      <c r="D16" s="5" t="inlineStr"/>
+      <c r="E16" s="5" t="inlineStr"/>
+      <c r="F16" s="5" t="inlineStr"/>
+      <c r="G16" s="5" t="inlineStr"/>
+      <c r="H16" s="5" t="inlineStr"/>
+      <c r="I16" s="5" t="inlineStr"/>
+      <c r="J16" s="5" t="inlineStr"/>
+      <c r="K16" s="5" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="inlineStr">
@@ -1065,14 +1058,10 @@
       </c>
       <c r="B17" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C17" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr"/>
       <c r="D17" s="5" t="inlineStr"/>
       <c r="E17" s="5" t="inlineStr"/>
       <c r="F17" s="5" t="inlineStr"/>
@@ -1095,7 +1084,7 @@
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>1.1.1.1.2.1.1</t>
         </is>
       </c>
       <c r="D18" s="7" t="inlineStr">
@@ -1140,7 +1129,7 @@
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>1.1.1.1.2.1.2</t>
         </is>
       </c>
       <c r="D19" s="7" t="inlineStr">
@@ -1185,7 +1174,7 @@
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>1.1.1.1.2.1.3</t>
         </is>
       </c>
       <c r="D20" s="7" t="inlineStr">
@@ -1218,44 +1207,40 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11" t="inlineStr">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                Battery Capacity</t>
         </is>
       </c>
-      <c r="B21" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C21" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D21" s="11" t="inlineStr"/>
-      <c r="E21" s="11" t="inlineStr"/>
-      <c r="F21" s="11" t="inlineStr"/>
-      <c r="G21" s="11" t="inlineStr"/>
-      <c r="H21" s="11" t="inlineStr"/>
-      <c r="I21" s="11" t="inlineStr"/>
-      <c r="J21" s="11" t="inlineStr"/>
-      <c r="K21" s="11" t="inlineStr"/>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="inlineStr"/>
+      <c r="D21" s="5" t="inlineStr"/>
+      <c r="E21" s="5" t="inlineStr"/>
+      <c r="F21" s="5" t="inlineStr"/>
+      <c r="G21" s="5" t="inlineStr"/>
+      <c r="H21" s="5" t="inlineStr"/>
+      <c r="I21" s="5" t="inlineStr"/>
+      <c r="J21" s="5" t="inlineStr"/>
+      <c r="K21" s="5" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="12" t="inlineStr">
+      <c r="A22" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Power Requirements</t>
         </is>
       </c>
-      <c r="B22" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C22" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
+      <c r="B22" s="11" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C22" s="11" t="inlineStr">
+        <is>
+          <t>1.1.1.2.1</t>
         </is>
       </c>
       <c r="D22" s="7" t="inlineStr">
@@ -1283,28 +1268,28 @@
           <t>I</t>
         </is>
       </c>
-      <c r="I22" s="12" t="inlineStr"/>
-      <c r="J22" s="12" t="n">
+      <c r="I22" s="11" t="inlineStr"/>
+      <c r="J22" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K22" s="12" t="n">
+      <c r="K22" s="11" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="12" t="inlineStr">
+      <c r="A23" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Usage Duration</t>
         </is>
       </c>
-      <c r="B23" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C23" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
+      <c r="B23" s="11" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C23" s="11" t="inlineStr">
+        <is>
+          <t>1.1.1.2.2</t>
         </is>
       </c>
       <c r="D23" s="7" t="inlineStr">
@@ -1332,28 +1317,28 @@
           <t>I</t>
         </is>
       </c>
-      <c r="I23" s="12" t="inlineStr"/>
-      <c r="J23" s="12" t="n">
+      <c r="I23" s="11" t="inlineStr"/>
+      <c r="J23" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K23" s="12" t="n">
+      <c r="K23" s="11" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="A24" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Size Constraints</t>
         </is>
       </c>
-      <c r="B24" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C24" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
+      <c r="B24" s="11" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C24" s="11" t="inlineStr">
+        <is>
+          <t>1.1.1.2.3</t>
         </is>
       </c>
       <c r="D24" s="7" t="inlineStr">
@@ -1366,7 +1351,7 @@
           <t>L</t>
         </is>
       </c>
-      <c r="F24" s="12" t="inlineStr"/>
+      <c r="F24" s="11" t="inlineStr"/>
       <c r="G24" s="9" t="inlineStr">
         <is>
           <t>P</t>
@@ -1377,53 +1362,49 @@
           <t>I</t>
         </is>
       </c>
-      <c r="I24" s="12" t="inlineStr"/>
-      <c r="J24" s="12" t="n">
+      <c r="I24" s="11" t="inlineStr"/>
+      <c r="J24" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K24" s="12" t="n">
+      <c r="K24" s="11" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="11" t="inlineStr">
+      <c r="A25" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                Battery Safety</t>
         </is>
       </c>
-      <c r="B25" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C25" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D25" s="11" t="inlineStr"/>
-      <c r="E25" s="11" t="inlineStr"/>
-      <c r="F25" s="11" t="inlineStr"/>
-      <c r="G25" s="11" t="inlineStr"/>
-      <c r="H25" s="11" t="inlineStr"/>
-      <c r="I25" s="11" t="inlineStr"/>
-      <c r="J25" s="11" t="inlineStr"/>
-      <c r="K25" s="11" t="inlineStr"/>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr"/>
+      <c r="D25" s="5" t="inlineStr"/>
+      <c r="E25" s="5" t="inlineStr"/>
+      <c r="F25" s="5" t="inlineStr"/>
+      <c r="G25" s="5" t="inlineStr"/>
+      <c r="H25" s="5" t="inlineStr"/>
+      <c r="I25" s="5" t="inlineStr"/>
+      <c r="J25" s="5" t="inlineStr"/>
+      <c r="K25" s="5" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="12" t="inlineStr">
+      <c r="A26" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Temperature Control</t>
         </is>
       </c>
-      <c r="B26" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C26" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
+      <c r="B26" s="11" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C26" s="11" t="inlineStr">
+        <is>
+          <t>1.1.1.3.1</t>
         </is>
       </c>
       <c r="D26" s="7" t="inlineStr">
@@ -1451,28 +1432,28 @@
           <t>I</t>
         </is>
       </c>
-      <c r="I26" s="12" t="inlineStr"/>
-      <c r="J26" s="12" t="n">
+      <c r="I26" s="11" t="inlineStr"/>
+      <c r="J26" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K26" s="12" t="n">
+      <c r="K26" s="11" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="12" t="inlineStr">
+      <c r="A27" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Protection Circuits</t>
         </is>
       </c>
-      <c r="B27" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C27" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
+      <c r="B27" s="11" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C27" s="11" t="inlineStr">
+        <is>
+          <t>1.1.1.3.2</t>
         </is>
       </c>
       <c r="D27" s="7" t="inlineStr">
@@ -1500,28 +1481,28 @@
           <t>I</t>
         </is>
       </c>
-      <c r="I27" s="12" t="inlineStr"/>
-      <c r="J27" s="12" t="n">
+      <c r="I27" s="11" t="inlineStr"/>
+      <c r="J27" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K27" s="12" t="n">
+      <c r="K27" s="11" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="12" t="inlineStr">
+      <c r="A28" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Certification Requirements</t>
         </is>
       </c>
-      <c r="B28" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C28" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
+      <c r="B28" s="11" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C28" s="11" t="inlineStr">
+        <is>
+          <t>1.1.1.3.3</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
@@ -1534,7 +1515,7 @@
           <t>P</t>
         </is>
       </c>
-      <c r="F28" s="12" t="inlineStr"/>
+      <c r="F28" s="11" t="inlineStr"/>
       <c r="G28" s="9" t="inlineStr">
         <is>
           <t>P</t>
@@ -1545,53 +1526,49 @@
           <t>I</t>
         </is>
       </c>
-      <c r="I28" s="12" t="inlineStr"/>
-      <c r="J28" s="12" t="n">
+      <c r="I28" s="11" t="inlineStr"/>
+      <c r="J28" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K28" s="12" t="n">
+      <c r="K28" s="11" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="11" t="inlineStr">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                Battery Suppliers</t>
         </is>
       </c>
-      <c r="B29" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C29" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D29" s="11" t="inlineStr"/>
-      <c r="E29" s="11" t="inlineStr"/>
-      <c r="F29" s="11" t="inlineStr"/>
-      <c r="G29" s="11" t="inlineStr"/>
-      <c r="H29" s="11" t="inlineStr"/>
-      <c r="I29" s="11" t="inlineStr"/>
-      <c r="J29" s="11" t="inlineStr"/>
-      <c r="K29" s="11" t="inlineStr"/>
+      <c r="B29" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C29" s="5" t="inlineStr"/>
+      <c r="D29" s="5" t="inlineStr"/>
+      <c r="E29" s="5" t="inlineStr"/>
+      <c r="F29" s="5" t="inlineStr"/>
+      <c r="G29" s="5" t="inlineStr"/>
+      <c r="H29" s="5" t="inlineStr"/>
+      <c r="I29" s="5" t="inlineStr"/>
+      <c r="J29" s="5" t="inlineStr"/>
+      <c r="K29" s="5" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="12" t="inlineStr">
+      <c r="A30" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Vendor Selection</t>
         </is>
       </c>
-      <c r="B30" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C30" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
+      <c r="B30" s="11" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C30" s="11" t="inlineStr">
+        <is>
+          <t>1.1.1.4.1</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
@@ -1604,102 +1581,98 @@
           <t>P</t>
         </is>
       </c>
-      <c r="F30" s="12" t="inlineStr"/>
-      <c r="G30" s="12" t="inlineStr"/>
+      <c r="F30" s="11" t="inlineStr"/>
+      <c r="G30" s="11" t="inlineStr"/>
       <c r="H30" s="10" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I30" s="12" t="inlineStr"/>
-      <c r="J30" s="12" t="n">
+      <c r="I30" s="11" t="inlineStr"/>
+      <c r="J30" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K30" s="12" t="n">
+      <c r="K30" s="11" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="inlineStr">
+      <c r="A31" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Plastic Research</t>
         </is>
       </c>
-      <c r="B31" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C31" s="4" t="inlineStr"/>
-      <c r="D31" s="4" t="inlineStr"/>
-      <c r="E31" s="4" t="inlineStr"/>
-      <c r="F31" s="4" t="inlineStr"/>
-      <c r="G31" s="4" t="inlineStr"/>
-      <c r="H31" s="4" t="inlineStr"/>
-      <c r="I31" s="4" t="inlineStr"/>
-      <c r="J31" s="4" t="inlineStr"/>
-      <c r="K31" s="4" t="inlineStr"/>
+      <c r="B31" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C31" s="5" t="inlineStr"/>
+      <c r="D31" s="5" t="inlineStr"/>
+      <c r="E31" s="5" t="inlineStr"/>
+      <c r="F31" s="5" t="inlineStr"/>
+      <c r="G31" s="5" t="inlineStr"/>
+      <c r="H31" s="5" t="inlineStr"/>
+      <c r="I31" s="5" t="inlineStr"/>
+      <c r="J31" s="5" t="inlineStr"/>
+      <c r="K31" s="5" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="inlineStr">
+      <c r="A32" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                Plastic Types</t>
         </is>
       </c>
-      <c r="B32" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C32" s="4" t="inlineStr"/>
-      <c r="D32" s="4" t="inlineStr"/>
-      <c r="E32" s="4" t="inlineStr"/>
-      <c r="F32" s="4" t="inlineStr"/>
-      <c r="G32" s="4" t="inlineStr"/>
-      <c r="H32" s="4" t="inlineStr"/>
-      <c r="I32" s="4" t="inlineStr"/>
-      <c r="J32" s="4" t="inlineStr"/>
-      <c r="K32" s="4" t="inlineStr"/>
+      <c r="B32" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C32" s="5" t="inlineStr"/>
+      <c r="D32" s="5" t="inlineStr"/>
+      <c r="E32" s="5" t="inlineStr"/>
+      <c r="F32" s="5" t="inlineStr"/>
+      <c r="G32" s="5" t="inlineStr"/>
+      <c r="H32" s="5" t="inlineStr"/>
+      <c r="I32" s="5" t="inlineStr"/>
+      <c r="J32" s="5" t="inlineStr"/>
+      <c r="K32" s="5" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="12" t="inlineStr">
+      <c r="A33" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    ABS Analysis</t>
         </is>
       </c>
-      <c r="B33" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C33" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D33" s="12" t="inlineStr"/>
-      <c r="E33" s="12" t="inlineStr"/>
-      <c r="F33" s="12" t="inlineStr"/>
-      <c r="G33" s="12" t="inlineStr"/>
-      <c r="H33" s="12" t="inlineStr"/>
-      <c r="I33" s="12" t="inlineStr"/>
-      <c r="J33" s="12" t="inlineStr"/>
-      <c r="K33" s="12" t="inlineStr"/>
+      <c r="B33" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C33" s="5" t="inlineStr"/>
+      <c r="D33" s="5" t="inlineStr"/>
+      <c r="E33" s="5" t="inlineStr"/>
+      <c r="F33" s="5" t="inlineStr"/>
+      <c r="G33" s="5" t="inlineStr"/>
+      <c r="H33" s="5" t="inlineStr"/>
+      <c r="I33" s="5" t="inlineStr"/>
+      <c r="J33" s="5" t="inlineStr"/>
+      <c r="K33" s="5" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" s="5" t="inlineStr">
+      <c r="A34" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">                        Impact Resistance</t>
         </is>
       </c>
-      <c r="B34" s="5" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C34" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
+      <c r="B34" s="12" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C34" s="12" t="inlineStr">
+        <is>
+          <t>1.1.2.1.1.1</t>
         </is>
       </c>
       <c r="D34" s="7" t="inlineStr">
@@ -1712,35 +1685,35 @@
           <t>L</t>
         </is>
       </c>
-      <c r="F34" s="5" t="inlineStr"/>
+      <c r="F34" s="12" t="inlineStr"/>
       <c r="G34" s="9" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H34" s="5" t="inlineStr"/>
-      <c r="I34" s="5" t="inlineStr"/>
-      <c r="J34" s="5" t="n">
+      <c r="H34" s="12" t="inlineStr"/>
+      <c r="I34" s="12" t="inlineStr"/>
+      <c r="J34" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="K34" s="5" t="n">
+      <c r="K34" s="12" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="5" t="inlineStr">
+      <c r="A35" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">                        Heat Resistance</t>
         </is>
       </c>
-      <c r="B35" s="5" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C35" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
+      <c r="B35" s="12" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C35" s="12" t="inlineStr">
+        <is>
+          <t>1.1.2.1.1.2</t>
         </is>
       </c>
       <c r="D35" s="7" t="inlineStr">
@@ -1753,35 +1726,35 @@
           <t>L</t>
         </is>
       </c>
-      <c r="F35" s="5" t="inlineStr"/>
+      <c r="F35" s="12" t="inlineStr"/>
       <c r="G35" s="9" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H35" s="5" t="inlineStr"/>
-      <c r="I35" s="5" t="inlineStr"/>
-      <c r="J35" s="5" t="n">
+      <c r="H35" s="12" t="inlineStr"/>
+      <c r="I35" s="12" t="inlineStr"/>
+      <c r="J35" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="K35" s="5" t="n">
+      <c r="K35" s="12" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="5" t="inlineStr">
+      <c r="A36" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">                        Cost Analysis</t>
         </is>
       </c>
-      <c r="B36" s="5" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C36" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
+      <c r="B36" s="12" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C36" s="12" t="inlineStr">
+        <is>
+          <t>1.1.2.1.1.3</t>
         </is>
       </c>
       <c r="D36" s="8" t="inlineStr">
@@ -1794,60 +1767,56 @@
           <t>P</t>
         </is>
       </c>
-      <c r="F36" s="5" t="inlineStr"/>
-      <c r="G36" s="5" t="inlineStr"/>
+      <c r="F36" s="12" t="inlineStr"/>
+      <c r="G36" s="12" t="inlineStr"/>
       <c r="H36" s="10" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I36" s="5" t="inlineStr"/>
-      <c r="J36" s="5" t="n">
+      <c r="I36" s="12" t="inlineStr"/>
+      <c r="J36" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="K36" s="5" t="n">
+      <c r="K36" s="12" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="12" t="inlineStr">
+      <c r="A37" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Polycarbonate Study</t>
         </is>
       </c>
-      <c r="B37" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C37" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D37" s="12" t="inlineStr"/>
-      <c r="E37" s="12" t="inlineStr"/>
-      <c r="F37" s="12" t="inlineStr"/>
-      <c r="G37" s="12" t="inlineStr"/>
-      <c r="H37" s="12" t="inlineStr"/>
-      <c r="I37" s="12" t="inlineStr"/>
-      <c r="J37" s="12" t="inlineStr"/>
-      <c r="K37" s="12" t="inlineStr"/>
+      <c r="B37" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C37" s="5" t="inlineStr"/>
+      <c r="D37" s="5" t="inlineStr"/>
+      <c r="E37" s="5" t="inlineStr"/>
+      <c r="F37" s="5" t="inlineStr"/>
+      <c r="G37" s="5" t="inlineStr"/>
+      <c r="H37" s="5" t="inlineStr"/>
+      <c r="I37" s="5" t="inlineStr"/>
+      <c r="J37" s="5" t="inlineStr"/>
+      <c r="K37" s="5" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" s="5" t="inlineStr">
+      <c r="A38" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">                        Durability Tests</t>
         </is>
       </c>
-      <c r="B38" s="5" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C38" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
+      <c r="B38" s="12" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C38" s="12" t="inlineStr">
+        <is>
+          <t>1.1.2.1.2.1</t>
         </is>
       </c>
       <c r="D38" s="7" t="inlineStr">
@@ -1860,35 +1829,35 @@
           <t>L</t>
         </is>
       </c>
-      <c r="F38" s="5" t="inlineStr"/>
+      <c r="F38" s="12" t="inlineStr"/>
       <c r="G38" s="9" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H38" s="5" t="inlineStr"/>
-      <c r="I38" s="5" t="inlineStr"/>
-      <c r="J38" s="5" t="n">
+      <c r="H38" s="12" t="inlineStr"/>
+      <c r="I38" s="12" t="inlineStr"/>
+      <c r="J38" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="K38" s="5" t="n">
+      <c r="K38" s="12" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="inlineStr">
+      <c r="A39" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">                        UV Resistance</t>
         </is>
       </c>
-      <c r="B39" s="5" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C39" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
+      <c r="B39" s="12" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C39" s="12" t="inlineStr">
+        <is>
+          <t>1.1.2.1.2.2</t>
         </is>
       </c>
       <c r="D39" s="7" t="inlineStr">
@@ -1901,35 +1870,35 @@
           <t>L</t>
         </is>
       </c>
-      <c r="F39" s="5" t="inlineStr"/>
+      <c r="F39" s="12" t="inlineStr"/>
       <c r="G39" s="9" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H39" s="5" t="inlineStr"/>
-      <c r="I39" s="5" t="inlineStr"/>
-      <c r="J39" s="5" t="n">
+      <c r="H39" s="12" t="inlineStr"/>
+      <c r="I39" s="12" t="inlineStr"/>
+      <c r="J39" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="K39" s="5" t="n">
+      <c r="K39" s="12" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="5" t="inlineStr">
+      <c r="A40" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">                        Manufacturing Process</t>
         </is>
       </c>
-      <c r="B40" s="5" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C40" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
+      <c r="B40" s="12" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C40" s="12" t="inlineStr">
+        <is>
+          <t>1.1.2.1.2.3</t>
         </is>
       </c>
       <c r="D40" s="7" t="inlineStr">
@@ -1942,7 +1911,7 @@
           <t>L</t>
         </is>
       </c>
-      <c r="F40" s="5" t="inlineStr"/>
+      <c r="F40" s="12" t="inlineStr"/>
       <c r="G40" s="9" t="inlineStr">
         <is>
           <t>P</t>
@@ -1953,11 +1922,11 @@
           <t>I</t>
         </is>
       </c>
-      <c r="I40" s="5" t="inlineStr"/>
-      <c r="J40" s="5" t="n">
+      <c r="I40" s="12" t="inlineStr"/>
+      <c r="J40" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="K40" s="5" t="n">
+      <c r="K40" s="12" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1983,44 +1952,40 @@
       <c r="K41" s="4" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" s="13" t="inlineStr">
+      <c r="A42" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Target Audience Research</t>
         </is>
       </c>
-      <c r="B42" s="13" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C42" s="13" t="inlineStr">
-        <is>
-          <t>1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D42" s="13" t="inlineStr"/>
-      <c r="E42" s="13" t="inlineStr"/>
-      <c r="F42" s="13" t="inlineStr"/>
-      <c r="G42" s="13" t="inlineStr"/>
-      <c r="H42" s="13" t="inlineStr"/>
-      <c r="I42" s="13" t="inlineStr"/>
-      <c r="J42" s="13" t="inlineStr"/>
-      <c r="K42" s="13" t="inlineStr"/>
+      <c r="B42" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C42" s="5" t="inlineStr"/>
+      <c r="D42" s="5" t="inlineStr"/>
+      <c r="E42" s="5" t="inlineStr"/>
+      <c r="F42" s="5" t="inlineStr"/>
+      <c r="G42" s="5" t="inlineStr"/>
+      <c r="H42" s="5" t="inlineStr"/>
+      <c r="I42" s="5" t="inlineStr"/>
+      <c r="J42" s="5" t="inlineStr"/>
+      <c r="K42" s="5" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" s="11" t="inlineStr">
+      <c r="A43" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Demographics</t>
         </is>
       </c>
-      <c r="B43" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C43" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B43" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C43" s="13" t="inlineStr">
+        <is>
+          <t>1.2.1.1</t>
         </is>
       </c>
       <c r="D43" s="8" t="inlineStr">
@@ -2028,9 +1993,9 @@
           <t>L</t>
         </is>
       </c>
-      <c r="E43" s="11" t="inlineStr"/>
-      <c r="F43" s="11" t="inlineStr"/>
-      <c r="G43" s="11" t="inlineStr"/>
+      <c r="E43" s="13" t="inlineStr"/>
+      <c r="F43" s="13" t="inlineStr"/>
+      <c r="G43" s="13" t="inlineStr"/>
       <c r="H43" s="10" t="inlineStr">
         <is>
           <t>I</t>
@@ -2041,27 +2006,27 @@
           <t>P</t>
         </is>
       </c>
-      <c r="J43" s="11" t="n">
+      <c r="J43" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="K43" s="11" t="n">
+      <c r="K43" s="13" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="11" t="inlineStr">
+      <c r="A44" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Usage Patterns</t>
         </is>
       </c>
-      <c r="B44" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C44" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B44" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C44" s="13" t="inlineStr">
+        <is>
+          <t>1.2.1.2</t>
         </is>
       </c>
       <c r="D44" s="8" t="inlineStr">
@@ -2069,9 +2034,9 @@
           <t>L</t>
         </is>
       </c>
-      <c r="E44" s="11" t="inlineStr"/>
-      <c r="F44" s="11" t="inlineStr"/>
-      <c r="G44" s="11" t="inlineStr"/>
+      <c r="E44" s="13" t="inlineStr"/>
+      <c r="F44" s="13" t="inlineStr"/>
+      <c r="G44" s="13" t="inlineStr"/>
       <c r="H44" s="10" t="inlineStr">
         <is>
           <t>I</t>
@@ -2082,27 +2047,27 @@
           <t>P</t>
         </is>
       </c>
-      <c r="J44" s="11" t="n">
+      <c r="J44" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="K44" s="11" t="n">
+      <c r="K44" s="13" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="11" t="inlineStr">
+      <c r="A45" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Purchase Behavior</t>
         </is>
       </c>
-      <c r="B45" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C45" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B45" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C45" s="13" t="inlineStr">
+        <is>
+          <t>1.2.1.3</t>
         </is>
       </c>
       <c r="D45" s="8" t="inlineStr">
@@ -2110,9 +2075,9 @@
           <t>L</t>
         </is>
       </c>
-      <c r="E45" s="11" t="inlineStr"/>
-      <c r="F45" s="11" t="inlineStr"/>
-      <c r="G45" s="11" t="inlineStr"/>
+      <c r="E45" s="13" t="inlineStr"/>
+      <c r="F45" s="13" t="inlineStr"/>
+      <c r="G45" s="13" t="inlineStr"/>
       <c r="H45" s="10" t="inlineStr">
         <is>
           <t>I</t>
@@ -2123,52 +2088,48 @@
           <t>P</t>
         </is>
       </c>
-      <c r="J45" s="11" t="n">
+      <c r="J45" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="K45" s="11" t="n">
+      <c r="K45" s="13" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="13" t="inlineStr">
+      <c r="A46" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            User Pain Points</t>
         </is>
       </c>
-      <c r="B46" s="13" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C46" s="13" t="inlineStr">
-        <is>
-          <t>1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D46" s="13" t="inlineStr"/>
-      <c r="E46" s="13" t="inlineStr"/>
-      <c r="F46" s="13" t="inlineStr"/>
-      <c r="G46" s="13" t="inlineStr"/>
-      <c r="H46" s="13" t="inlineStr"/>
-      <c r="I46" s="13" t="inlineStr"/>
-      <c r="J46" s="13" t="inlineStr"/>
-      <c r="K46" s="13" t="inlineStr"/>
+      <c r="B46" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C46" s="5" t="inlineStr"/>
+      <c r="D46" s="5" t="inlineStr"/>
+      <c r="E46" s="5" t="inlineStr"/>
+      <c r="F46" s="5" t="inlineStr"/>
+      <c r="G46" s="5" t="inlineStr"/>
+      <c r="H46" s="5" t="inlineStr"/>
+      <c r="I46" s="5" t="inlineStr"/>
+      <c r="J46" s="5" t="inlineStr"/>
+      <c r="K46" s="5" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" s="11" t="inlineStr">
+      <c r="A47" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Current Solutions</t>
         </is>
       </c>
-      <c r="B47" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C47" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B47" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C47" s="13" t="inlineStr">
+        <is>
+          <t>1.2.2.1</t>
         </is>
       </c>
       <c r="D47" s="8" t="inlineStr">
@@ -2186,34 +2147,34 @@
           <t>P</t>
         </is>
       </c>
-      <c r="G47" s="11" t="inlineStr"/>
+      <c r="G47" s="13" t="inlineStr"/>
       <c r="H47" s="10" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I47" s="11" t="inlineStr"/>
-      <c r="J47" s="11" t="n">
+      <c r="I47" s="13" t="inlineStr"/>
+      <c r="J47" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="K47" s="11" t="n">
+      <c r="K47" s="13" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="11" t="inlineStr">
+      <c r="A48" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Unmet Needs</t>
         </is>
       </c>
-      <c r="B48" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C48" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B48" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C48" s="13" t="inlineStr">
+        <is>
+          <t>1.2.2.2</t>
         </is>
       </c>
       <c r="D48" s="8" t="inlineStr">
@@ -2231,34 +2192,34 @@
           <t>P</t>
         </is>
       </c>
-      <c r="G48" s="11" t="inlineStr"/>
+      <c r="G48" s="13" t="inlineStr"/>
       <c r="H48" s="10" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I48" s="11" t="inlineStr"/>
-      <c r="J48" s="11" t="n">
+      <c r="I48" s="13" t="inlineStr"/>
+      <c r="J48" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="K48" s="11" t="n">
+      <c r="K48" s="13" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="11" t="inlineStr">
+      <c r="A49" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Feature Requests</t>
         </is>
       </c>
-      <c r="B49" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C49" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B49" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C49" s="13" t="inlineStr">
+        <is>
+          <t>1.2.2.3</t>
         </is>
       </c>
       <c r="D49" s="8" t="inlineStr">
@@ -2276,17 +2237,17 @@
           <t>P</t>
         </is>
       </c>
-      <c r="G49" s="11" t="inlineStr"/>
+      <c r="G49" s="13" t="inlineStr"/>
       <c r="H49" s="10" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I49" s="11" t="inlineStr"/>
-      <c r="J49" s="11" t="n">
+      <c r="I49" s="13" t="inlineStr"/>
+      <c r="J49" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="K49" s="11" t="n">
+      <c r="K49" s="13" t="n">
         <v>16</v>
       </c>
     </row>
@@ -2333,44 +2294,40 @@
       <c r="K51" s="4" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" s="13" t="inlineStr">
+      <c r="A52" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Battery Procurement</t>
         </is>
       </c>
-      <c r="B52" s="13" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C52" s="13" t="inlineStr">
-        <is>
-          <t>1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D52" s="13" t="inlineStr"/>
-      <c r="E52" s="13" t="inlineStr"/>
-      <c r="F52" s="13" t="inlineStr"/>
-      <c r="G52" s="13" t="inlineStr"/>
-      <c r="H52" s="13" t="inlineStr"/>
-      <c r="I52" s="13" t="inlineStr"/>
-      <c r="J52" s="13" t="inlineStr"/>
-      <c r="K52" s="13" t="inlineStr"/>
+      <c r="B52" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C52" s="5" t="inlineStr"/>
+      <c r="D52" s="5" t="inlineStr"/>
+      <c r="E52" s="5" t="inlineStr"/>
+      <c r="F52" s="5" t="inlineStr"/>
+      <c r="G52" s="5" t="inlineStr"/>
+      <c r="H52" s="5" t="inlineStr"/>
+      <c r="I52" s="5" t="inlineStr"/>
+      <c r="J52" s="5" t="inlineStr"/>
+      <c r="K52" s="5" t="inlineStr"/>
     </row>
     <row r="53">
-      <c r="A53" s="11" t="inlineStr">
+      <c r="A53" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Supplier Selection</t>
         </is>
       </c>
-      <c r="B53" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C53" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B53" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C53" s="13" t="inlineStr">
+        <is>
+          <t>2.1.1.1</t>
         </is>
       </c>
       <c r="D53" s="8" t="inlineStr">
@@ -2383,35 +2340,35 @@
           <t>P</t>
         </is>
       </c>
-      <c r="F53" s="11" t="inlineStr"/>
-      <c r="G53" s="11" t="inlineStr"/>
+      <c r="F53" s="13" t="inlineStr"/>
+      <c r="G53" s="13" t="inlineStr"/>
       <c r="H53" s="10" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I53" s="11" t="inlineStr"/>
-      <c r="J53" s="11" t="n">
+      <c r="I53" s="13" t="inlineStr"/>
+      <c r="J53" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="K53" s="11" t="n">
+      <c r="K53" s="13" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="11" t="inlineStr">
+      <c r="A54" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Quality Verification</t>
         </is>
       </c>
-      <c r="B54" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C54" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B54" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C54" s="13" t="inlineStr">
+        <is>
+          <t>2.1.1.2</t>
         </is>
       </c>
       <c r="D54" s="7" t="inlineStr">
@@ -2424,35 +2381,35 @@
           <t>L</t>
         </is>
       </c>
-      <c r="F54" s="11" t="inlineStr"/>
+      <c r="F54" s="13" t="inlineStr"/>
       <c r="G54" s="9" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H54" s="11" t="inlineStr"/>
-      <c r="I54" s="11" t="inlineStr"/>
-      <c r="J54" s="11" t="n">
+      <c r="H54" s="13" t="inlineStr"/>
+      <c r="I54" s="13" t="inlineStr"/>
+      <c r="J54" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="K54" s="11" t="n">
+      <c r="K54" s="13" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="11" t="inlineStr">
+      <c r="A55" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Cost Negotiation</t>
         </is>
       </c>
-      <c r="B55" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C55" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B55" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C55" s="13" t="inlineStr">
+        <is>
+          <t>2.1.1.3</t>
         </is>
       </c>
       <c r="D55" s="8" t="inlineStr">
@@ -2465,60 +2422,56 @@
           <t>P</t>
         </is>
       </c>
-      <c r="F55" s="11" t="inlineStr"/>
-      <c r="G55" s="11" t="inlineStr"/>
+      <c r="F55" s="13" t="inlineStr"/>
+      <c r="G55" s="13" t="inlineStr"/>
       <c r="H55" s="10" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I55" s="11" t="inlineStr"/>
-      <c r="J55" s="11" t="n">
+      <c r="I55" s="13" t="inlineStr"/>
+      <c r="J55" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="K55" s="11" t="n">
+      <c r="K55" s="13" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="13" t="inlineStr">
+      <c r="A56" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Electronics Components</t>
         </is>
       </c>
-      <c r="B56" s="13" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C56" s="13" t="inlineStr">
-        <is>
-          <t>1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D56" s="13" t="inlineStr"/>
-      <c r="E56" s="13" t="inlineStr"/>
-      <c r="F56" s="13" t="inlineStr"/>
-      <c r="G56" s="13" t="inlineStr"/>
-      <c r="H56" s="13" t="inlineStr"/>
-      <c r="I56" s="13" t="inlineStr"/>
-      <c r="J56" s="13" t="inlineStr"/>
-      <c r="K56" s="13" t="inlineStr"/>
+      <c r="B56" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C56" s="5" t="inlineStr"/>
+      <c r="D56" s="5" t="inlineStr"/>
+      <c r="E56" s="5" t="inlineStr"/>
+      <c r="F56" s="5" t="inlineStr"/>
+      <c r="G56" s="5" t="inlineStr"/>
+      <c r="H56" s="5" t="inlineStr"/>
+      <c r="I56" s="5" t="inlineStr"/>
+      <c r="J56" s="5" t="inlineStr"/>
+      <c r="K56" s="5" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" s="11" t="inlineStr">
+      <c r="A57" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Component List</t>
         </is>
       </c>
-      <c r="B57" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C57" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B57" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C57" s="13" t="inlineStr">
+        <is>
+          <t>2.1.2.1</t>
         </is>
       </c>
       <c r="D57" s="7" t="inlineStr">
@@ -2536,30 +2489,30 @@
           <t>P</t>
         </is>
       </c>
-      <c r="G57" s="11" t="inlineStr"/>
-      <c r="H57" s="11" t="inlineStr"/>
-      <c r="I57" s="11" t="inlineStr"/>
-      <c r="J57" s="11" t="n">
+      <c r="G57" s="13" t="inlineStr"/>
+      <c r="H57" s="13" t="inlineStr"/>
+      <c r="I57" s="13" t="inlineStr"/>
+      <c r="J57" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="K57" s="11" t="n">
+      <c r="K57" s="13" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="11" t="inlineStr">
+      <c r="A58" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Supplier Quotes</t>
         </is>
       </c>
-      <c r="B58" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C58" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B58" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C58" s="13" t="inlineStr">
+        <is>
+          <t>2.1.2.2</t>
         </is>
       </c>
       <c r="D58" s="8" t="inlineStr">
@@ -2572,35 +2525,35 @@
           <t>P</t>
         </is>
       </c>
-      <c r="F58" s="11" t="inlineStr"/>
-      <c r="G58" s="11" t="inlineStr"/>
+      <c r="F58" s="13" t="inlineStr"/>
+      <c r="G58" s="13" t="inlineStr"/>
       <c r="H58" s="10" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I58" s="11" t="inlineStr"/>
-      <c r="J58" s="11" t="n">
+      <c r="I58" s="13" t="inlineStr"/>
+      <c r="J58" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="K58" s="11" t="n">
+      <c r="K58" s="13" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="11" t="inlineStr">
+      <c r="A59" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Lead Time Analysis</t>
         </is>
       </c>
-      <c r="B59" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C59" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B59" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C59" s="13" t="inlineStr">
+        <is>
+          <t>2.1.2.3</t>
         </is>
       </c>
       <c r="D59" s="8" t="inlineStr">
@@ -2613,18 +2566,18 @@
           <t>P</t>
         </is>
       </c>
-      <c r="F59" s="11" t="inlineStr"/>
-      <c r="G59" s="11" t="inlineStr"/>
+      <c r="F59" s="13" t="inlineStr"/>
+      <c r="G59" s="13" t="inlineStr"/>
       <c r="H59" s="10" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="I59" s="11" t="inlineStr"/>
-      <c r="J59" s="11" t="n">
+      <c r="I59" s="13" t="inlineStr"/>
+      <c r="J59" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="K59" s="11" t="n">
+      <c r="K59" s="13" t="n">
         <v>16</v>
       </c>
     </row>
@@ -2650,44 +2603,40 @@
       <c r="K60" s="4" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" s="13" t="inlineStr">
+      <c r="A61" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Initial Prototype</t>
         </is>
       </c>
-      <c r="B61" s="13" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C61" s="13" t="inlineStr">
-        <is>
-          <t>1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D61" s="13" t="inlineStr"/>
-      <c r="E61" s="13" t="inlineStr"/>
-      <c r="F61" s="13" t="inlineStr"/>
-      <c r="G61" s="13" t="inlineStr"/>
-      <c r="H61" s="13" t="inlineStr"/>
-      <c r="I61" s="13" t="inlineStr"/>
-      <c r="J61" s="13" t="inlineStr"/>
-      <c r="K61" s="13" t="inlineStr"/>
+      <c r="B61" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C61" s="5" t="inlineStr"/>
+      <c r="D61" s="5" t="inlineStr"/>
+      <c r="E61" s="5" t="inlineStr"/>
+      <c r="F61" s="5" t="inlineStr"/>
+      <c r="G61" s="5" t="inlineStr"/>
+      <c r="H61" s="5" t="inlineStr"/>
+      <c r="I61" s="5" t="inlineStr"/>
+      <c r="J61" s="5" t="inlineStr"/>
+      <c r="K61" s="5" t="inlineStr"/>
     </row>
     <row r="62">
-      <c r="A62" s="11" t="inlineStr">
+      <c r="A62" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                3D Printing</t>
         </is>
       </c>
-      <c r="B62" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C62" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B62" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C62" s="13" t="inlineStr">
+        <is>
+          <t>2.2.1.1</t>
         </is>
       </c>
       <c r="D62" s="7" t="inlineStr">
@@ -2700,35 +2649,35 @@
           <t>L</t>
         </is>
       </c>
-      <c r="F62" s="11" t="inlineStr"/>
+      <c r="F62" s="13" t="inlineStr"/>
       <c r="G62" s="9" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="H62" s="11" t="inlineStr"/>
-      <c r="I62" s="11" t="inlineStr"/>
-      <c r="J62" s="11" t="n">
+      <c r="H62" s="13" t="inlineStr"/>
+      <c r="I62" s="13" t="inlineStr"/>
+      <c r="J62" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="K62" s="11" t="n">
+      <c r="K62" s="13" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="11" t="inlineStr">
+      <c r="A63" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Assembly</t>
         </is>
       </c>
-      <c r="B63" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C63" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B63" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C63" s="13" t="inlineStr">
+        <is>
+          <t>2.2.1.2</t>
         </is>
       </c>
       <c r="D63" s="7" t="inlineStr">
@@ -2751,29 +2700,29 @@
           <t>P</t>
         </is>
       </c>
-      <c r="H63" s="11" t="inlineStr"/>
-      <c r="I63" s="11" t="inlineStr"/>
-      <c r="J63" s="11" t="n">
+      <c r="H63" s="13" t="inlineStr"/>
+      <c r="I63" s="13" t="inlineStr"/>
+      <c r="J63" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="K63" s="11" t="n">
+      <c r="K63" s="13" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="11" t="inlineStr">
+      <c r="A64" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Testing</t>
         </is>
       </c>
-      <c r="B64" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C64" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B64" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C64" s="13" t="inlineStr">
+        <is>
+          <t>2.2.1.3</t>
         </is>
       </c>
       <c r="D64" s="7" t="inlineStr">
@@ -2796,54 +2745,50 @@
           <t>L</t>
         </is>
       </c>
-      <c r="H64" s="11" t="inlineStr"/>
-      <c r="I64" s="11" t="inlineStr"/>
-      <c r="J64" s="11" t="n">
+      <c r="H64" s="13" t="inlineStr"/>
+      <c r="I64" s="13" t="inlineStr"/>
+      <c r="J64" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="K64" s="11" t="n">
+      <c r="K64" s="13" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="13" t="inlineStr">
+      <c r="A65" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Final Prototype</t>
         </is>
       </c>
-      <c r="B65" s="13" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C65" s="13" t="inlineStr">
-        <is>
-          <t>1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D65" s="13" t="inlineStr"/>
-      <c r="E65" s="13" t="inlineStr"/>
-      <c r="F65" s="13" t="inlineStr"/>
-      <c r="G65" s="13" t="inlineStr"/>
-      <c r="H65" s="13" t="inlineStr"/>
-      <c r="I65" s="13" t="inlineStr"/>
-      <c r="J65" s="13" t="inlineStr"/>
-      <c r="K65" s="13" t="inlineStr"/>
+      <c r="B65" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C65" s="5" t="inlineStr"/>
+      <c r="D65" s="5" t="inlineStr"/>
+      <c r="E65" s="5" t="inlineStr"/>
+      <c r="F65" s="5" t="inlineStr"/>
+      <c r="G65" s="5" t="inlineStr"/>
+      <c r="H65" s="5" t="inlineStr"/>
+      <c r="I65" s="5" t="inlineStr"/>
+      <c r="J65" s="5" t="inlineStr"/>
+      <c r="K65" s="5" t="inlineStr"/>
     </row>
     <row r="66">
-      <c r="A66" s="11" t="inlineStr">
+      <c r="A66" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Production Methods</t>
         </is>
       </c>
-      <c r="B66" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C66" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B66" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C66" s="13" t="inlineStr">
+        <is>
+          <t>2.2.2.1</t>
         </is>
       </c>
       <c r="D66" s="8" t="inlineStr">
@@ -2856,7 +2801,7 @@
           <t>P</t>
         </is>
       </c>
-      <c r="F66" s="11" t="inlineStr"/>
+      <c r="F66" s="13" t="inlineStr"/>
       <c r="G66" s="9" t="inlineStr">
         <is>
           <t>P</t>
@@ -2867,28 +2812,28 @@
           <t>I</t>
         </is>
       </c>
-      <c r="I66" s="11" t="inlineStr"/>
-      <c r="J66" s="11" t="n">
+      <c r="I66" s="13" t="inlineStr"/>
+      <c r="J66" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="K66" s="11" t="n">
+      <c r="K66" s="13" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="11" t="inlineStr">
+      <c r="A67" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Quality Control</t>
         </is>
       </c>
-      <c r="B67" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C67" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B67" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C67" s="13" t="inlineStr">
+        <is>
+          <t>2.2.2.2</t>
         </is>
       </c>
       <c r="D67" s="7" t="inlineStr">
@@ -2901,35 +2846,35 @@
           <t>P</t>
         </is>
       </c>
-      <c r="F67" s="11" t="inlineStr"/>
+      <c r="F67" s="13" t="inlineStr"/>
       <c r="G67" s="8" t="inlineStr">
         <is>
           <t>L</t>
         </is>
       </c>
-      <c r="H67" s="11" t="inlineStr"/>
-      <c r="I67" s="11" t="inlineStr"/>
-      <c r="J67" s="11" t="n">
+      <c r="H67" s="13" t="inlineStr"/>
+      <c r="I67" s="13" t="inlineStr"/>
+      <c r="J67" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="K67" s="11" t="n">
+      <c r="K67" s="13" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="11" t="inlineStr">
+      <c r="A68" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">                Documentation</t>
         </is>
       </c>
-      <c r="B68" s="11" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C68" s="11" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1</t>
+      <c r="B68" s="13" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C68" s="13" t="inlineStr">
+        <is>
+          <t>2.2.2.3</t>
         </is>
       </c>
       <c r="D68" s="8" t="inlineStr">
@@ -2957,11 +2902,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="I68" s="11" t="inlineStr"/>
-      <c r="J68" s="11" t="n">
+      <c r="I68" s="13" t="inlineStr"/>
+      <c r="J68" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="K68" s="11" t="n">
+      <c r="K68" s="13" t="n">
         <v>24</v>
       </c>
     </row>
@@ -3008,67 +2953,67 @@
       <c r="K70" s="4" t="inlineStr"/>
     </row>
     <row r="71">
-      <c r="A71" s="4" t="inlineStr">
+      <c r="A71" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Component Testing</t>
         </is>
       </c>
-      <c r="B71" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C71" s="4" t="inlineStr"/>
-      <c r="D71" s="4" t="inlineStr"/>
-      <c r="E71" s="4" t="inlineStr"/>
-      <c r="F71" s="4" t="inlineStr"/>
-      <c r="G71" s="4" t="inlineStr"/>
-      <c r="H71" s="4" t="inlineStr"/>
-      <c r="I71" s="4" t="inlineStr"/>
-      <c r="J71" s="4" t="inlineStr"/>
-      <c r="K71" s="4" t="inlineStr"/>
+      <c r="B71" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C71" s="5" t="inlineStr"/>
+      <c r="D71" s="5" t="inlineStr"/>
+      <c r="E71" s="5" t="inlineStr"/>
+      <c r="F71" s="5" t="inlineStr"/>
+      <c r="G71" s="5" t="inlineStr"/>
+      <c r="H71" s="5" t="inlineStr"/>
+      <c r="I71" s="5" t="inlineStr"/>
+      <c r="J71" s="5" t="inlineStr"/>
+      <c r="K71" s="5" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" s="4" t="inlineStr">
+      <c r="A72" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                Electrical Testing</t>
         </is>
       </c>
-      <c r="B72" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C72" s="4" t="inlineStr"/>
-      <c r="D72" s="4" t="inlineStr"/>
-      <c r="E72" s="4" t="inlineStr"/>
-      <c r="F72" s="4" t="inlineStr"/>
-      <c r="G72" s="4" t="inlineStr"/>
-      <c r="H72" s="4" t="inlineStr"/>
-      <c r="I72" s="4" t="inlineStr"/>
-      <c r="J72" s="4" t="inlineStr"/>
-      <c r="K72" s="4" t="inlineStr"/>
+      <c r="B72" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C72" s="5" t="inlineStr"/>
+      <c r="D72" s="5" t="inlineStr"/>
+      <c r="E72" s="5" t="inlineStr"/>
+      <c r="F72" s="5" t="inlineStr"/>
+      <c r="G72" s="5" t="inlineStr"/>
+      <c r="H72" s="5" t="inlineStr"/>
+      <c r="I72" s="5" t="inlineStr"/>
+      <c r="J72" s="5" t="inlineStr"/>
+      <c r="K72" s="5" t="inlineStr"/>
     </row>
     <row r="73">
-      <c r="A73" s="4" t="inlineStr">
+      <c r="A73" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Power System</t>
         </is>
       </c>
-      <c r="B73" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C73" s="4" t="inlineStr"/>
-      <c r="D73" s="4" t="inlineStr"/>
-      <c r="E73" s="4" t="inlineStr"/>
-      <c r="F73" s="4" t="inlineStr"/>
-      <c r="G73" s="4" t="inlineStr"/>
-      <c r="H73" s="4" t="inlineStr"/>
-      <c r="I73" s="4" t="inlineStr"/>
-      <c r="J73" s="4" t="inlineStr"/>
-      <c r="K73" s="4" t="inlineStr"/>
+      <c r="B73" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C73" s="5" t="inlineStr"/>
+      <c r="D73" s="5" t="inlineStr"/>
+      <c r="E73" s="5" t="inlineStr"/>
+      <c r="F73" s="5" t="inlineStr"/>
+      <c r="G73" s="5" t="inlineStr"/>
+      <c r="H73" s="5" t="inlineStr"/>
+      <c r="I73" s="5" t="inlineStr"/>
+      <c r="J73" s="5" t="inlineStr"/>
+      <c r="K73" s="5" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="5" t="inlineStr">
@@ -3078,14 +3023,10 @@
       </c>
       <c r="B74" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C74" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C74" s="5" t="inlineStr"/>
       <c r="D74" s="5" t="inlineStr"/>
       <c r="E74" s="5" t="inlineStr"/>
       <c r="F74" s="5" t="inlineStr"/>
@@ -3108,7 +3049,7 @@
       </c>
       <c r="C75" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>3.1.1.1.1.1.1</t>
         </is>
       </c>
       <c r="D75" s="7" t="inlineStr">
@@ -3149,7 +3090,7 @@
       </c>
       <c r="C76" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>3.1.1.1.1.1.2</t>
         </is>
       </c>
       <c r="D76" s="7" t="inlineStr">
@@ -3190,7 +3131,7 @@
       </c>
       <c r="C77" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>3.1.1.1.1.1.3</t>
         </is>
       </c>
       <c r="D77" s="7" t="inlineStr">
@@ -3226,14 +3167,10 @@
       </c>
       <c r="B78" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C78" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C78" s="5" t="inlineStr"/>
       <c r="D78" s="5" t="inlineStr"/>
       <c r="E78" s="5" t="inlineStr"/>
       <c r="F78" s="5" t="inlineStr"/>
@@ -3256,7 +3193,7 @@
       </c>
       <c r="C79" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>3.1.1.1.1.2.1</t>
         </is>
       </c>
       <c r="D79" s="7" t="inlineStr">
@@ -3301,7 +3238,7 @@
       </c>
       <c r="C80" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>3.1.1.1.1.2.2</t>
         </is>
       </c>
       <c r="D80" s="7" t="inlineStr">
@@ -3342,7 +3279,7 @@
       </c>
       <c r="C81" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>3.1.1.1.1.2.3</t>
         </is>
       </c>
       <c r="D81" s="7" t="inlineStr">
@@ -3371,25 +3308,25 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="4" t="inlineStr">
+      <c r="A82" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Control System</t>
         </is>
       </c>
-      <c r="B82" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C82" s="4" t="inlineStr"/>
-      <c r="D82" s="4" t="inlineStr"/>
-      <c r="E82" s="4" t="inlineStr"/>
-      <c r="F82" s="4" t="inlineStr"/>
-      <c r="G82" s="4" t="inlineStr"/>
-      <c r="H82" s="4" t="inlineStr"/>
-      <c r="I82" s="4" t="inlineStr"/>
-      <c r="J82" s="4" t="inlineStr"/>
-      <c r="K82" s="4" t="inlineStr"/>
+      <c r="B82" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C82" s="5" t="inlineStr"/>
+      <c r="D82" s="5" t="inlineStr"/>
+      <c r="E82" s="5" t="inlineStr"/>
+      <c r="F82" s="5" t="inlineStr"/>
+      <c r="G82" s="5" t="inlineStr"/>
+      <c r="H82" s="5" t="inlineStr"/>
+      <c r="I82" s="5" t="inlineStr"/>
+      <c r="J82" s="5" t="inlineStr"/>
+      <c r="K82" s="5" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="5" t="inlineStr">
@@ -3399,14 +3336,10 @@
       </c>
       <c r="B83" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C83" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C83" s="5" t="inlineStr"/>
       <c r="D83" s="5" t="inlineStr"/>
       <c r="E83" s="5" t="inlineStr"/>
       <c r="F83" s="5" t="inlineStr"/>
@@ -3429,7 +3362,7 @@
       </c>
       <c r="C84" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>3.1.1.1.2.1.1</t>
         </is>
       </c>
       <c r="D84" s="7" t="inlineStr">
@@ -3474,7 +3407,7 @@
       </c>
       <c r="C85" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>3.1.1.1.2.1.2</t>
         </is>
       </c>
       <c r="D85" s="7" t="inlineStr">
@@ -3519,7 +3452,7 @@
       </c>
       <c r="C86" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>3.1.1.1.2.1.3</t>
         </is>
       </c>
       <c r="D86" s="7" t="inlineStr">
@@ -3594,67 +3527,67 @@
       <c r="K88" s="4" t="inlineStr"/>
     </row>
     <row r="89">
-      <c r="A89" s="4" t="inlineStr">
+      <c r="A89" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Social Media</t>
         </is>
       </c>
-      <c r="B89" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C89" s="4" t="inlineStr"/>
-      <c r="D89" s="4" t="inlineStr"/>
-      <c r="E89" s="4" t="inlineStr"/>
-      <c r="F89" s="4" t="inlineStr"/>
-      <c r="G89" s="4" t="inlineStr"/>
-      <c r="H89" s="4" t="inlineStr"/>
-      <c r="I89" s="4" t="inlineStr"/>
-      <c r="J89" s="4" t="inlineStr"/>
-      <c r="K89" s="4" t="inlineStr"/>
+      <c r="B89" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C89" s="5" t="inlineStr"/>
+      <c r="D89" s="5" t="inlineStr"/>
+      <c r="E89" s="5" t="inlineStr"/>
+      <c r="F89" s="5" t="inlineStr"/>
+      <c r="G89" s="5" t="inlineStr"/>
+      <c r="H89" s="5" t="inlineStr"/>
+      <c r="I89" s="5" t="inlineStr"/>
+      <c r="J89" s="5" t="inlineStr"/>
+      <c r="K89" s="5" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" s="4" t="inlineStr">
+      <c r="A90" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                Platform Strategy</t>
         </is>
       </c>
-      <c r="B90" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C90" s="4" t="inlineStr"/>
-      <c r="D90" s="4" t="inlineStr"/>
-      <c r="E90" s="4" t="inlineStr"/>
-      <c r="F90" s="4" t="inlineStr"/>
-      <c r="G90" s="4" t="inlineStr"/>
-      <c r="H90" s="4" t="inlineStr"/>
-      <c r="I90" s="4" t="inlineStr"/>
-      <c r="J90" s="4" t="inlineStr"/>
-      <c r="K90" s="4" t="inlineStr"/>
+      <c r="B90" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C90" s="5" t="inlineStr"/>
+      <c r="D90" s="5" t="inlineStr"/>
+      <c r="E90" s="5" t="inlineStr"/>
+      <c r="F90" s="5" t="inlineStr"/>
+      <c r="G90" s="5" t="inlineStr"/>
+      <c r="H90" s="5" t="inlineStr"/>
+      <c r="I90" s="5" t="inlineStr"/>
+      <c r="J90" s="5" t="inlineStr"/>
+      <c r="K90" s="5" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" s="4" t="inlineStr">
+      <c r="A91" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Instagram Campaign</t>
         </is>
       </c>
-      <c r="B91" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C91" s="4" t="inlineStr"/>
-      <c r="D91" s="4" t="inlineStr"/>
-      <c r="E91" s="4" t="inlineStr"/>
-      <c r="F91" s="4" t="inlineStr"/>
-      <c r="G91" s="4" t="inlineStr"/>
-      <c r="H91" s="4" t="inlineStr"/>
-      <c r="I91" s="4" t="inlineStr"/>
-      <c r="J91" s="4" t="inlineStr"/>
-      <c r="K91" s="4" t="inlineStr"/>
+      <c r="B91" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C91" s="5" t="inlineStr"/>
+      <c r="D91" s="5" t="inlineStr"/>
+      <c r="E91" s="5" t="inlineStr"/>
+      <c r="F91" s="5" t="inlineStr"/>
+      <c r="G91" s="5" t="inlineStr"/>
+      <c r="H91" s="5" t="inlineStr"/>
+      <c r="I91" s="5" t="inlineStr"/>
+      <c r="J91" s="5" t="inlineStr"/>
+      <c r="K91" s="5" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="5" t="inlineStr">
@@ -3664,14 +3597,10 @@
       </c>
       <c r="B92" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C92" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C92" s="5" t="inlineStr"/>
       <c r="D92" s="5" t="inlineStr"/>
       <c r="E92" s="5" t="inlineStr"/>
       <c r="F92" s="5" t="inlineStr"/>
@@ -3694,7 +3623,7 @@
       </c>
       <c r="C93" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>4.1.1.1.1.1.1</t>
         </is>
       </c>
       <c r="D93" s="7" t="inlineStr">
@@ -3735,7 +3664,7 @@
       </c>
       <c r="C94" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>4.1.1.1.1.1.2</t>
         </is>
       </c>
       <c r="D94" s="7" t="inlineStr">
@@ -3776,7 +3705,7 @@
       </c>
       <c r="C95" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>4.1.1.1.1.1.3</t>
         </is>
       </c>
       <c r="D95" s="7" t="inlineStr">
@@ -3812,14 +3741,10 @@
       </c>
       <c r="B96" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C96" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C96" s="5" t="inlineStr"/>
       <c r="D96" s="5" t="inlineStr"/>
       <c r="E96" s="5" t="inlineStr"/>
       <c r="F96" s="5" t="inlineStr"/>
@@ -3842,7 +3767,7 @@
       </c>
       <c r="C97" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>4.1.1.1.1.2.1</t>
         </is>
       </c>
       <c r="D97" s="8" t="inlineStr">
@@ -3883,7 +3808,7 @@
       </c>
       <c r="C98" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>4.1.1.1.1.2.2</t>
         </is>
       </c>
       <c r="D98" s="8" t="inlineStr">
@@ -3928,7 +3853,7 @@
       </c>
       <c r="C99" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>4.1.1.1.1.2.3</t>
         </is>
       </c>
       <c r="D99" s="8" t="inlineStr">
@@ -3961,44 +3886,40 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="12" t="inlineStr">
+      <c r="A100" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    TikTok Strategy</t>
         </is>
       </c>
-      <c r="B100" s="12" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C100" s="12" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1</t>
-        </is>
-      </c>
-      <c r="D100" s="12" t="inlineStr"/>
-      <c r="E100" s="12" t="inlineStr"/>
-      <c r="F100" s="12" t="inlineStr"/>
-      <c r="G100" s="12" t="inlineStr"/>
-      <c r="H100" s="12" t="inlineStr"/>
-      <c r="I100" s="12" t="inlineStr"/>
-      <c r="J100" s="12" t="inlineStr"/>
-      <c r="K100" s="12" t="inlineStr"/>
+      <c r="B100" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C100" s="5" t="inlineStr"/>
+      <c r="D100" s="5" t="inlineStr"/>
+      <c r="E100" s="5" t="inlineStr"/>
+      <c r="F100" s="5" t="inlineStr"/>
+      <c r="G100" s="5" t="inlineStr"/>
+      <c r="H100" s="5" t="inlineStr"/>
+      <c r="I100" s="5" t="inlineStr"/>
+      <c r="J100" s="5" t="inlineStr"/>
+      <c r="K100" s="5" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" s="5" t="inlineStr">
+      <c r="A101" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">                        Trend Analysis</t>
         </is>
       </c>
-      <c r="B101" s="5" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C101" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
+      <c r="B101" s="12" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C101" s="12" t="inlineStr">
+        <is>
+          <t>4.1.1.1.2.1</t>
         </is>
       </c>
       <c r="D101" s="7" t="inlineStr">
@@ -4006,9 +3927,9 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E101" s="5" t="inlineStr"/>
-      <c r="F101" s="5" t="inlineStr"/>
-      <c r="G101" s="5" t="inlineStr"/>
+      <c r="E101" s="12" t="inlineStr"/>
+      <c r="F101" s="12" t="inlineStr"/>
+      <c r="G101" s="12" t="inlineStr"/>
       <c r="H101" s="10" t="inlineStr">
         <is>
           <t>I</t>
@@ -4019,27 +3940,27 @@
           <t>L</t>
         </is>
       </c>
-      <c r="J101" s="5" t="n">
+      <c r="J101" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="K101" s="5" t="n">
+      <c r="K101" s="12" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="5" t="inlineStr">
+      <c r="A102" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">                        Content Calendar</t>
         </is>
       </c>
-      <c r="B102" s="5" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C102" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
+      <c r="B102" s="12" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C102" s="12" t="inlineStr">
+        <is>
+          <t>4.1.1.1.2.2</t>
         </is>
       </c>
       <c r="D102" s="7" t="inlineStr">
@@ -4047,9 +3968,9 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E102" s="5" t="inlineStr"/>
-      <c r="F102" s="5" t="inlineStr"/>
-      <c r="G102" s="5" t="inlineStr"/>
+      <c r="E102" s="12" t="inlineStr"/>
+      <c r="F102" s="12" t="inlineStr"/>
+      <c r="G102" s="12" t="inlineStr"/>
       <c r="H102" s="10" t="inlineStr">
         <is>
           <t>I</t>
@@ -4060,27 +3981,27 @@
           <t>L</t>
         </is>
       </c>
-      <c r="J102" s="5" t="n">
+      <c r="J102" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="K102" s="5" t="n">
+      <c r="K102" s="12" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="5" t="inlineStr">
+      <c r="A103" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">                        Performance Metrics</t>
         </is>
       </c>
-      <c r="B103" s="5" t="inlineStr">
-        <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C103" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
+      <c r="B103" s="12" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="C103" s="12" t="inlineStr">
+        <is>
+          <t>4.1.1.1.2.3</t>
         </is>
       </c>
       <c r="D103" s="7" t="inlineStr">
@@ -4088,13 +4009,13 @@
           <t>R</t>
         </is>
       </c>
-      <c r="E103" s="5" t="inlineStr"/>
+      <c r="E103" s="12" t="inlineStr"/>
       <c r="F103" s="9" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="G103" s="5" t="inlineStr"/>
+      <c r="G103" s="12" t="inlineStr"/>
       <c r="H103" s="10" t="inlineStr">
         <is>
           <t>I</t>
@@ -4105,10 +4026,10 @@
           <t>L</t>
         </is>
       </c>
-      <c r="J103" s="5" t="n">
+      <c r="J103" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="K103" s="5" t="n">
+      <c r="K103" s="12" t="n">
         <v>16</v>
       </c>
     </row>
@@ -4155,67 +4076,67 @@
       <c r="K105" s="4" t="inlineStr"/>
     </row>
     <row r="106">
-      <c r="A106" s="4" t="inlineStr">
+      <c r="A106" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">            Assembly Line Design</t>
         </is>
       </c>
-      <c r="B106" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C106" s="4" t="inlineStr"/>
-      <c r="D106" s="4" t="inlineStr"/>
-      <c r="E106" s="4" t="inlineStr"/>
-      <c r="F106" s="4" t="inlineStr"/>
-      <c r="G106" s="4" t="inlineStr"/>
-      <c r="H106" s="4" t="inlineStr"/>
-      <c r="I106" s="4" t="inlineStr"/>
-      <c r="J106" s="4" t="inlineStr"/>
-      <c r="K106" s="4" t="inlineStr"/>
+      <c r="B106" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C106" s="5" t="inlineStr"/>
+      <c r="D106" s="5" t="inlineStr"/>
+      <c r="E106" s="5" t="inlineStr"/>
+      <c r="F106" s="5" t="inlineStr"/>
+      <c r="G106" s="5" t="inlineStr"/>
+      <c r="H106" s="5" t="inlineStr"/>
+      <c r="I106" s="5" t="inlineStr"/>
+      <c r="J106" s="5" t="inlineStr"/>
+      <c r="K106" s="5" t="inlineStr"/>
     </row>
     <row r="107">
-      <c r="A107" s="4" t="inlineStr">
+      <c r="A107" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                Automation Systems</t>
         </is>
       </c>
-      <c r="B107" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C107" s="4" t="inlineStr"/>
-      <c r="D107" s="4" t="inlineStr"/>
-      <c r="E107" s="4" t="inlineStr"/>
-      <c r="F107" s="4" t="inlineStr"/>
-      <c r="G107" s="4" t="inlineStr"/>
-      <c r="H107" s="4" t="inlineStr"/>
-      <c r="I107" s="4" t="inlineStr"/>
-      <c r="J107" s="4" t="inlineStr"/>
-      <c r="K107" s="4" t="inlineStr"/>
+      <c r="B107" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C107" s="5" t="inlineStr"/>
+      <c r="D107" s="5" t="inlineStr"/>
+      <c r="E107" s="5" t="inlineStr"/>
+      <c r="F107" s="5" t="inlineStr"/>
+      <c r="G107" s="5" t="inlineStr"/>
+      <c r="H107" s="5" t="inlineStr"/>
+      <c r="I107" s="5" t="inlineStr"/>
+      <c r="J107" s="5" t="inlineStr"/>
+      <c r="K107" s="5" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" s="4" t="inlineStr">
+      <c r="A108" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Robot Integration</t>
         </is>
       </c>
-      <c r="B108" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C108" s="4" t="inlineStr"/>
-      <c r="D108" s="4" t="inlineStr"/>
-      <c r="E108" s="4" t="inlineStr"/>
-      <c r="F108" s="4" t="inlineStr"/>
-      <c r="G108" s="4" t="inlineStr"/>
-      <c r="H108" s="4" t="inlineStr"/>
-      <c r="I108" s="4" t="inlineStr"/>
-      <c r="J108" s="4" t="inlineStr"/>
-      <c r="K108" s="4" t="inlineStr"/>
+      <c r="B108" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C108" s="5" t="inlineStr"/>
+      <c r="D108" s="5" t="inlineStr"/>
+      <c r="E108" s="5" t="inlineStr"/>
+      <c r="F108" s="5" t="inlineStr"/>
+      <c r="G108" s="5" t="inlineStr"/>
+      <c r="H108" s="5" t="inlineStr"/>
+      <c r="I108" s="5" t="inlineStr"/>
+      <c r="J108" s="5" t="inlineStr"/>
+      <c r="K108" s="5" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="5" t="inlineStr">
@@ -4225,14 +4146,10 @@
       </c>
       <c r="B109" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C109" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C109" s="5" t="inlineStr"/>
       <c r="D109" s="5" t="inlineStr"/>
       <c r="E109" s="5" t="inlineStr"/>
       <c r="F109" s="5" t="inlineStr"/>
@@ -4255,7 +4172,7 @@
       </c>
       <c r="C110" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>5.1.1.1.1.1.1</t>
         </is>
       </c>
       <c r="D110" s="7" t="inlineStr">
@@ -4300,7 +4217,7 @@
       </c>
       <c r="C111" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>5.1.1.1.1.1.2</t>
         </is>
       </c>
       <c r="D111" s="7" t="inlineStr">
@@ -4345,7 +4262,7 @@
       </c>
       <c r="C112" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>5.1.1.1.1.1.3</t>
         </is>
       </c>
       <c r="D112" s="7" t="inlineStr">
@@ -4385,14 +4302,10 @@
       </c>
       <c r="B113" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C113" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C113" s="5" t="inlineStr"/>
       <c r="D113" s="5" t="inlineStr"/>
       <c r="E113" s="5" t="inlineStr"/>
       <c r="F113" s="5" t="inlineStr"/>
@@ -4415,7 +4328,7 @@
       </c>
       <c r="C114" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>5.1.1.1.1.2.1</t>
         </is>
       </c>
       <c r="D114" s="7" t="inlineStr">
@@ -4460,7 +4373,7 @@
       </c>
       <c r="C115" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>5.1.1.1.1.2.2</t>
         </is>
       </c>
       <c r="D115" s="7" t="inlineStr">
@@ -4505,7 +4418,7 @@
       </c>
       <c r="C116" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>5.1.1.1.1.2.3</t>
         </is>
       </c>
       <c r="D116" s="7" t="inlineStr">
@@ -4538,25 +4451,25 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="4" t="inlineStr">
+      <c r="A117" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">                    Vision System</t>
         </is>
       </c>
-      <c r="B117" s="4" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="C117" s="4" t="inlineStr"/>
-      <c r="D117" s="4" t="inlineStr"/>
-      <c r="E117" s="4" t="inlineStr"/>
-      <c r="F117" s="4" t="inlineStr"/>
-      <c r="G117" s="4" t="inlineStr"/>
-      <c r="H117" s="4" t="inlineStr"/>
-      <c r="I117" s="4" t="inlineStr"/>
-      <c r="J117" s="4" t="inlineStr"/>
-      <c r="K117" s="4" t="inlineStr"/>
+      <c r="B117" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C117" s="5" t="inlineStr"/>
+      <c r="D117" s="5" t="inlineStr"/>
+      <c r="E117" s="5" t="inlineStr"/>
+      <c r="F117" s="5" t="inlineStr"/>
+      <c r="G117" s="5" t="inlineStr"/>
+      <c r="H117" s="5" t="inlineStr"/>
+      <c r="I117" s="5" t="inlineStr"/>
+      <c r="J117" s="5" t="inlineStr"/>
+      <c r="K117" s="5" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="5" t="inlineStr">
@@ -4566,14 +4479,10 @@
       </c>
       <c r="B118" s="5" t="inlineStr">
         <is>
-          <t>Subtask</t>
-        </is>
-      </c>
-      <c r="C118" s="5" t="inlineStr">
-        <is>
-          <t>1.1.1.1.1.1.1</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C118" s="5" t="inlineStr"/>
       <c r="D118" s="5" t="inlineStr"/>
       <c r="E118" s="5" t="inlineStr"/>
       <c r="F118" s="5" t="inlineStr"/>
@@ -4596,7 +4505,7 @@
       </c>
       <c r="C119" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>5.1.1.1.2.1.1</t>
         </is>
       </c>
       <c r="D119" s="7" t="inlineStr">
@@ -4641,7 +4550,7 @@
       </c>
       <c r="C120" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>5.1.1.1.2.1.2</t>
         </is>
       </c>
       <c r="D120" s="7" t="inlineStr">
@@ -4686,7 +4595,7 @@
       </c>
       <c r="C121" s="6" t="inlineStr">
         <is>
-          <t>1.1.1.1.1.1.1.1</t>
+          <t>5.1.1.1.2.1.3</t>
         </is>
       </c>
       <c r="D121" s="7" t="inlineStr">
@@ -4734,7 +4643,7 @@
     <row r="124">
       <c r="A124" s="15" t="inlineStr">
         <is>
-          <t>Total WBS Boxes:</t>
+          <t>Total Items:</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -4775,7 +4684,12 @@
           <t>Activity</t>
         </is>
       </c>
-      <c r="K124" s="16" t="inlineStr">
+      <c r="K124" s="5" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="L124" s="16" t="inlineStr">
         <is>
           <t>Subtask*</t>
         </is>
@@ -4803,17 +4717,47 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="15" t="inlineStr">
         <is>
+          <t>Total Tasks:</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="15" t="inlineStr">
+        <is>
           <t>Total Work Packages:</t>
         </is>
       </c>
-      <c r="B127" t="n">
-        <v>90</v>
+      <c r="B128" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="15" t="inlineStr">
+        <is>
+          <t>Total Duration (Days):</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="15" t="inlineStr">
+        <is>
+          <t>Total Labor (Hours):</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>1480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>